<commit_message>
Final V1: Admin Mode & Luxury Login
</commit_message>
<xml_diff>
--- a/public/data/plan_tagging_fictif.xlsx
+++ b/public/data/plan_tagging_fictif.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,9 @@
       <c r="E1" t="str">
         <v>Description</v>
       </c>
+      <c r="F1" t="str">
+        <v>PHOTO</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -435,6 +438,9 @@
       <c r="E2" t="str">
         <v>User views a product</v>
       </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -452,6 +458,9 @@
       <c r="E3" t="str">
         <v>User adds item to cart</v>
       </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -469,6 +478,9 @@
       <c r="E4" t="str">
         <v>User removes item</v>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -486,6 +498,9 @@
       <c r="E5" t="str">
         <v>User starts checkout</v>
       </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -503,6 +518,9 @@
       <c r="E6" t="str">
         <v>Completed order</v>
       </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -520,6 +538,9 @@
       <c r="E7" t="str">
         <v>User performs search</v>
       </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -537,6 +558,9 @@
       <c r="E8" t="str">
         <v>User logs in</v>
       </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -554,6 +578,9 @@
       <c r="E9" t="str">
         <v>User signs up</v>
       </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -571,6 +598,9 @@
       <c r="E10" t="str">
         <v>User views cart</v>
       </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -588,10 +618,13 @@
       <c r="E11" t="str">
         <v>User selects item in list</v>
       </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>